<commit_message>
Python SOE matches format and conversation flow of Java sample
</commit_message>
<xml_diff>
--- a/soe/python/callerProfileAPI/callerProfile.xlsx
+++ b/soe/python/callerProfileAPI/callerProfile.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdcalus/dev/voicegateway/VoiceGatewayWatson-VoiceProxy/callerProfileAPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/workspace/sample.voice.gateway/soe/python/callerProfileAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="2940" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Olivia</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>gymnastics</t>
+  </si>
+  <si>
+    <t>mastercard</t>
+  </si>
+  <si>
+    <t>visa</t>
+  </si>
+  <si>
+    <t>discovercard</t>
+  </si>
+  <si>
+    <t>americanexpress</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,7 +431,7 @@
     <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -453,8 +465,20 @@
       <c r="K1" t="s">
         <v>16</v>
       </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -489,7 +513,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -524,7 +548,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -559,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -594,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>

</xml_diff>